<commit_message>
DSL is now always produced with "ng" for human and "cp" for templates (as opposed to "K cp"). Input excel can have empty rows.
</commit_message>
<xml_diff>
--- a/app/mob2dsl/user_input.xlsx
+++ b/app/mob2dsl/user_input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dnae969-my.sharepoint.com/personal/chris_icely_dnae_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\assay-screening-proj\app\mob2dsl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26C79DCC-8C6D-43BD-B8B1-AEF0E464549C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36BB839-F402-4AEC-B520-19139DEB802A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8616" activeTab="1" xr2:uid="{375B1353-46A6-4499-A08E-730321ABAAF1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="6516" xr2:uid="{375B1353-46A6-4499-A08E-730321ABAAF1}"/>
   </bookViews>
   <sheets>
     <sheet name="allocation" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="62">
   <si>
     <t>Plate</t>
   </si>
@@ -128,42 +128,6 @@
   </si>
   <si>
     <t>HgDNA_Promega305466</t>
-  </si>
-  <si>
-    <t>HgDNA_Promega305467</t>
-  </si>
-  <si>
-    <t>HgDNA_Promega305468</t>
-  </si>
-  <si>
-    <t>HgDNA_Promega305469</t>
-  </si>
-  <si>
-    <t>HgDNA_Promega305470</t>
-  </si>
-  <si>
-    <t>HgDNA_Promega305472</t>
-  </si>
-  <si>
-    <t>HgDNA_Promega305473</t>
-  </si>
-  <si>
-    <t>HgDNA_Promega305474</t>
-  </si>
-  <si>
-    <t>HgDNA_Promega305475</t>
-  </si>
-  <si>
-    <t>HgDNA_Promega305476</t>
-  </si>
-  <si>
-    <t>HgDNA_Promega305477</t>
-  </si>
-  <si>
-    <t>HgDNA_Promega305478</t>
-  </si>
-  <si>
-    <t>HgDNA_Promega305479</t>
   </si>
   <si>
     <t>Sample</t>
@@ -707,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4907F0-6D8C-48F0-BF43-395D1B0B7405}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,7 +742,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -796,7 +760,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -814,7 +778,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -832,7 +796,7 @@
         <v>9</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -846,151 +810,167 @@
       <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D9" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>26</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>27</v>
+        <v>10</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>29</v>
+        <v>13</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>29</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>27</v>
+        <v>18</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>29</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="A14" s="5"/>
       <c r="B14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E17" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="15" t="s">
-        <v>45</v>
+      <c r="F17" s="15" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1003,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEAA583D-AB59-4E18-8060-45F3725C7F75}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1015,371 +995,371 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="H1" s="17">
         <v>7</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="J1" s="17" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="L3" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="M3" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="M4" s="19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="J5" s="19" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="L5" s="19" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="M5" s="19" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="L6" s="19" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="M6" s="19" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="L7" s="19" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="M7" s="19" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="M8" s="19" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="M9" s="19" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>